<commit_message>
Created pbix and project snippets
</commit_message>
<xml_diff>
--- a/Data/events_criteria_tables.xlsx
+++ b/Data/events_criteria_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/755301589831b088/7. Portfolio Data Analytics/Challenges/Maven Analytics - Power Outage/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/755301589831b088/7. Portfolio Data Analytics/Challenges/Maven Analytics/Power-Outage-Challenge/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{C1D24FB7-69DB-4C61-8826-683EFE345263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2FA8FF6-4799-4CF9-A967-0CC24E1257FD}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{C1D24FB7-69DB-4C61-8826-683EFE345263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFA879F3-53AC-4CFF-BD02-829EEBDC3231}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="20" windowWidth="38620" windowHeight="21100" xr2:uid="{E4D615A7-C449-4B36-8E41-B28A2F7DBF8C}"/>
+    <workbookView xWindow="4590" yWindow="3770" windowWidth="28800" windowHeight="15320" activeTab="2" xr2:uid="{E4D615A7-C449-4B36-8E41-B28A2F7DBF8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Alert Criteria" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -248,7 +248,88 @@
     <t>Action Taken</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve"> Damage or destruction of its Facility that results from actual or suspected intentional human action.</t>
+  </si>
+  <si>
+    <t>Cause Short</t>
+  </si>
+  <si>
+    <t>Cyber event (information)</t>
+  </si>
+  <si>
+    <t>Cyber event (operational)</t>
+  </si>
+  <si>
+    <t>Fuel supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmission equipment failure </t>
+  </si>
+  <si>
+    <t>Failure at high voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator loss or failure </t>
+  </si>
+  <si>
+    <t>Action Taken Short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shed Firm Load </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public Appeal </t>
+  </si>
+  <si>
+    <t>Implemented warning etc.</t>
+  </si>
+  <si>
+    <t>Impact Short</t>
+  </si>
+  <si>
+    <t>Control center loss</t>
+  </si>
+  <si>
+    <t>Facility Damage</t>
+  </si>
+  <si>
+    <t>Control Center Communication</t>
+  </si>
+  <si>
+    <t>Electrical Separation</t>
+  </si>
+  <si>
+    <t>Complete Shutdown</t>
+  </si>
+  <si>
+    <t>Major Interruption</t>
+  </si>
+  <si>
+    <t>Major Interruption of +3 BES</t>
+  </si>
+  <si>
+    <t>Uncontrolled 200MW loss</t>
+  </si>
+  <si>
+    <t>Service Loss +50K customers</t>
+  </si>
+  <si>
+    <t>Voltage Reduction</t>
+  </si>
+  <si>
+    <t>Voltage Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inadequate resources </t>
+  </si>
+  <si>
+    <t>Cap. Loss + 1,400MW</t>
+  </si>
+  <si>
+    <t>Cap. Loss + 2,000MW</t>
+  </si>
+  <si>
+    <t>Loss Nuclear Generation</t>
   </si>
 </sst>
 </file>
@@ -622,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00D561C-337A-4A26-8A56-F86876E3E662}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -914,142 +995,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7E4943-89E2-4019-8A8B-DEFAA9B9A441}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="77.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1060,158 +1190,213 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D826DA53-B19D-4DB8-A252-B47092A82702}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="72.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1222,94 +1407,125 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA67BEB-0D61-45EC-9761-E29DD88B63C6}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="134.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>